<commit_message>
revised list of health centers
</commit_message>
<xml_diff>
--- a/Applications and selections  07-29-16.xlsx
+++ b/Applications and selections  07-29-16.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" tabRatio="500" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="All Applications" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Final Selections" sheetId="13" r:id="rId6"/>
     <sheet name="update 28 July 2016" sheetId="14" r:id="rId7"/>
     <sheet name="short_names" sheetId="15" r:id="rId8"/>
+    <sheet name="contactOctShiny" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3644" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3664" uniqueCount="1004">
   <si>
     <t>Clinic Name</t>
   </si>
@@ -3413,12 +3414,45 @@
   <si>
     <t>Nasson</t>
   </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>contact1</t>
+  </si>
+  <si>
+    <t>contact2</t>
+  </si>
+  <si>
+    <t>Mary's</t>
+  </si>
+  <si>
+    <t>Hometown</t>
+  </si>
+  <si>
+    <t>Sunshine</t>
+  </si>
+  <si>
+    <t>York County Nasson</t>
+  </si>
+  <si>
+    <t>jackie.nestle@sclhs.net</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>repaired columns S and R</t>
+  </si>
+  <si>
+    <t>Choptank</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3544,6 +3578,13 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF626262"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3767,7 +3808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4039,6 +4080,9 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7066,7 +7110,7 @@
       </c>
     </row>
     <row r="26" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="113" t="s">
+      <c r="A26" s="116" t="s">
         <v>605</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -7147,7 +7191,7 @@
       </c>
     </row>
     <row r="27" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="113"/>
+      <c r="A27" s="116"/>
       <c r="B27" s="9" t="s">
         <v>607</v>
       </c>
@@ -7214,7 +7258,7 @@
       <c r="AM27" s="63"/>
     </row>
     <row r="28" spans="1:39" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="113"/>
+      <c r="A28" s="116"/>
       <c r="B28" s="20" t="s">
         <v>608</v>
       </c>
@@ -7281,7 +7325,7 @@
       </c>
     </row>
     <row r="29" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="113"/>
+      <c r="A29" s="116"/>
       <c r="B29" s="9" t="s">
         <v>609</v>
       </c>
@@ -16672,7 +16716,7 @@
       </c>
     </row>
     <row r="4" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="117" t="s">
         <v>605</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -16753,7 +16797,7 @@
       </c>
     </row>
     <row r="5" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="115"/>
+      <c r="A5" s="118"/>
       <c r="B5" s="9" t="s">
         <v>909</v>
       </c>
@@ -16820,7 +16864,7 @@
       <c r="AM5" s="63"/>
     </row>
     <row r="6" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="115"/>
+      <c r="A6" s="118"/>
       <c r="B6" s="20" t="s">
         <v>910</v>
       </c>
@@ -16887,7 +16931,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="116"/>
+      <c r="A7" s="119"/>
       <c r="B7" s="9" t="s">
         <v>911</v>
       </c>
@@ -17034,7 +17078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="125" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -17648,26 +17692,26 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="117" t="s">
+      <c r="A22" s="120" t="s">
         <v>953</v>
       </c>
-      <c r="B22" s="118"/>
-      <c r="C22" s="118"/>
-      <c r="D22" s="118"/>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="119"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="121"/>
+      <c r="D22" s="121"/>
+      <c r="E22" s="121"/>
+      <c r="F22" s="121"/>
+      <c r="G22" s="121"/>
+      <c r="H22" s="122"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="120"/>
-      <c r="B23" s="121"/>
-      <c r="C23" s="121"/>
-      <c r="D23" s="121"/>
-      <c r="E23" s="121"/>
-      <c r="F23" s="121"/>
-      <c r="G23" s="121"/>
-      <c r="H23" s="122"/>
+      <c r="A23" s="123"/>
+      <c r="B23" s="124"/>
+      <c r="C23" s="124"/>
+      <c r="D23" s="124"/>
+      <c r="E23" s="124"/>
+      <c r="F23" s="124"/>
+      <c r="G23" s="124"/>
+      <c r="H23" s="125"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
@@ -17839,7 +17883,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18642,26 +18686,26 @@
       <c r="J27" s="96"/>
     </row>
     <row r="28" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="117" t="s">
+      <c r="A28" s="120" t="s">
         <v>953</v>
       </c>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="119"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="121"/>
+      <c r="D28" s="121"/>
+      <c r="E28" s="121"/>
+      <c r="F28" s="121"/>
+      <c r="G28" s="121"/>
+      <c r="H28" s="122"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="120"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="121"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
-      <c r="F29" s="121"/>
-      <c r="G29" s="121"/>
-      <c r="H29" s="122"/>
+      <c r="A29" s="123"/>
+      <c r="B29" s="124"/>
+      <c r="C29" s="124"/>
+      <c r="D29" s="124"/>
+      <c r="E29" s="124"/>
+      <c r="F29" s="124"/>
+      <c r="G29" s="124"/>
+      <c r="H29" s="125"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
@@ -18858,8 +18902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -19251,4 +19295,143 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.09765625" customWidth="1"/>
+    <col min="2" max="2" width="20.59765625" customWidth="1"/>
+    <col min="3" max="3" width="22.796875" customWidth="1"/>
+    <col min="4" max="4" width="25.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="57" t="s">
+        <v>993</v>
+      </c>
+      <c r="B1" s="57" t="s">
+        <v>994</v>
+      </c>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="57" t="s">
+        <v>996</v>
+      </c>
+      <c r="B2" s="114" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="57" t="s">
+        <v>997</v>
+      </c>
+      <c r="B4" s="114" t="s">
+        <v>179</v>
+      </c>
+      <c r="C4" s="57"/>
+      <c r="D4" s="57"/>
+      <c r="E4" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="57"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="57" t="s">
+        <v>936</v>
+      </c>
+      <c r="B6" s="115" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="57"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="57" t="s">
+        <v>998</v>
+      </c>
+      <c r="B8" s="114" t="s">
+        <v>598</v>
+      </c>
+      <c r="C8" s="57"/>
+      <c r="D8" s="114" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="57"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="57" t="s">
+        <v>999</v>
+      </c>
+      <c r="B10" s="113" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>878</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="D8" r:id="rId5"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="0" r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Excel files for clinic names and measures 27 Jan 2017
</commit_message>
<xml_diff>
--- a/Applications and selections  07-29-16.xlsx
+++ b/Applications and selections  07-29-16.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" tabRatio="500" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="All Applications" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3664" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3692" uniqueCount="1011">
   <si>
     <t>Clinic Name</t>
   </si>
@@ -3446,6 +3446,28 @@
   </si>
   <si>
     <t>Choptank</t>
+  </si>
+  <si>
+    <t>Community Health Center Franklin Cnty</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lakeshore Community Health Care</t>
+  </si>
+  <si>
+    <t>Short.Name.EJ</t>
+  </si>
+  <si>
+    <t>Community of Hope.Inc</t>
+  </si>
+  <si>
+    <t>Community Health Center of Richmond.Inc</t>
+  </si>
+  <si>
+    <t>Family Health Center of Marshfield.Inc</t>
+  </si>
+  <si>
+    <t>Mary's Center for Maternal and Child Care.Inc</t>
   </si>
 </sst>
 </file>
@@ -3808,7 +3830,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4103,6 +4125,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4382,7 +4407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4390,6 +4415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AM46"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
@@ -9109,6 +9135,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AL19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11141,6 +11168,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:AQ38"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -15574,6 +15602,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -16363,6 +16392,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:AM8"/>
   <sheetViews>
     <sheetView topLeftCell="W2" workbookViewId="0">
@@ -17076,6 +17106,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
@@ -17880,6 +17911,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18900,396 +18932,481 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <sheetPr codeName="Sheet8"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="53.796875" customWidth="1"/>
-    <col min="3" max="3" width="10.796875" customWidth="1"/>
+    <col min="1" max="3" width="53.796875" customWidth="1"/>
+    <col min="4" max="4" width="10.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="90" t="s">
         <v>978</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" s="53" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
         <v>921</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>963</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="38" t="s">
+        <v>921</v>
+      </c>
+      <c r="D2">
         <f>LEN(B2)</f>
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="51" t="s">
         <v>914</v>
       </c>
       <c r="B3" s="51" t="s">
         <v>977</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C27" si="0">LEN(B3)</f>
+      <c r="C3" s="51" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D27" si="0">LEN(B3)</f>
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="110" t="s">
         <v>979</v>
       </c>
       <c r="B4" s="109" t="s">
         <v>981</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="126" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="48" t="s">
         <v>964</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="48" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F5" s="126" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="110" t="s">
         <v>980</v>
       </c>
       <c r="B6" s="109" t="s">
         <v>982</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="126" t="s">
+        <v>980</v>
+      </c>
+      <c r="D6">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
         <v>941</v>
       </c>
       <c r="B7" s="109" t="s">
         <v>974</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="38" t="s">
+        <v>941</v>
+      </c>
+      <c r="D7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="48" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="48" t="s">
         <v>983</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="48" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D8">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="49" t="s">
         <v>976</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="48" t="s">
         <v>965</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="110" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="109" t="s">
         <v>984</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="126" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D12">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="38" t="s">
         <v>936</v>
       </c>
       <c r="B13" s="38" t="s">
         <v>936</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="38" t="s">
+        <v>936</v>
+      </c>
+      <c r="D13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="48" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="48" t="s">
         <v>967</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="111" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="109" t="s">
         <v>985</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="126" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="48" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
         <v>961</v>
       </c>
       <c r="B17" s="48" t="s">
         <v>966</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="110" t="s">
         <v>26</v>
       </c>
       <c r="B18" s="48" t="s">
         <v>878</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="126" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="48" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="48" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="48" t="s">
         <v>968</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="48" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="48" t="s">
         <v>969</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="110" t="s">
         <v>987</v>
       </c>
       <c r="B22" s="48" t="s">
         <v>988</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="126" t="s">
+        <v>987</v>
+      </c>
+      <c r="D22">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="112" t="s">
         <v>990</v>
       </c>
       <c r="B23" s="109" t="s">
         <v>986</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="126" t="s">
+        <v>990</v>
+      </c>
+      <c r="D23">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="48" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="48" t="s">
         <v>970</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="38" t="s">
         <v>946</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>971</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="38" t="s">
+        <v>946</v>
+      </c>
+      <c r="D25">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="52" t="s">
         <v>991</v>
       </c>
       <c r="B26" s="52" t="s">
         <v>992</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="52" t="s">
+        <v>991</v>
+      </c>
+      <c r="D26">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="48" t="s">
         <v>37</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>973</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B28" s="108"/>
     </row>
   </sheetData>
@@ -19299,9 +19416,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -19432,6 +19550,6 @@
     <hyperlink ref="D8" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="0" r:id="rId6"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
edits to the input spreadsheet
</commit_message>
<xml_diff>
--- a/Applications and selections  07-29-16.xlsx
+++ b/Applications and selections  07-29-16.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9516" tabRatio="500" firstSheet="5" activeTab="7"/>
@@ -18,16 +18,12 @@
     <sheet name="contactOctShiny" sheetId="16" r:id="rId9"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3692" uniqueCount="1011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3693" uniqueCount="1012">
   <si>
     <t>Clinic Name</t>
   </si>
@@ -3468,6 +3464,9 @@
   </si>
   <si>
     <t>Mary's Center for Maternal and Child Care.Inc</t>
+  </si>
+  <si>
+    <t>Check name</t>
   </si>
 </sst>
 </file>
@@ -3610,7 +3609,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3662,6 +3661,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3830,7 +3835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -4105,6 +4110,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -4125,9 +4134,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4144,9 +4150,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -6916,7 +6919,7 @@
         <v>602</v>
       </c>
       <c r="C24" s="66">
-        <f t="shared" ref="C24" si="0">SUM(C26:C29)</f>
+        <f>SUM(C26:C29)</f>
         <v>1</v>
       </c>
       <c r="D24" s="66">
@@ -6924,143 +6927,143 @@
         <v>2</v>
       </c>
       <c r="E24" s="66">
-        <f t="shared" ref="E24:AM24" si="1">SUM(E25:E30)</f>
+        <f t="shared" ref="E24:AM24" si="0">SUM(E25:E30)</f>
         <v>2</v>
       </c>
       <c r="F24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="G24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="M24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
       <c r="O24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="P24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="Q24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="S24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="T24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="U24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="V24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="W24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="X24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Y24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Z24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AB24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AC24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="AD24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AE24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AF24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AG24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AI24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AJ24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AK24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AL24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="AM24" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -7136,7 +7139,7 @@
       </c>
     </row>
     <row r="26" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="116" t="s">
+      <c r="A26" s="118" t="s">
         <v>605</v>
       </c>
       <c r="B26" s="9" t="s">
@@ -7217,7 +7220,7 @@
       </c>
     </row>
     <row r="27" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="116"/>
+      <c r="A27" s="118"/>
       <c r="B27" s="9" t="s">
         <v>607</v>
       </c>
@@ -7284,7 +7287,7 @@
       <c r="AM27" s="63"/>
     </row>
     <row r="28" spans="1:39" s="23" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="116"/>
+      <c r="A28" s="118"/>
       <c r="B28" s="20" t="s">
         <v>608</v>
       </c>
@@ -7351,7 +7354,7 @@
       </c>
     </row>
     <row r="29" spans="1:39" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="116"/>
+      <c r="A29" s="118"/>
       <c r="B29" s="9" t="s">
         <v>609</v>
       </c>
@@ -9125,11 +9128,6 @@
     <hyperlink ref="AF23" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -11158,11 +11156,6 @@
     <hyperlink ref="W16" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -15592,11 +15585,6 @@
     <hyperlink ref="X31" r:id="rId36"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -16382,11 +16370,6 @@
   </sortState>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -16526,7 +16509,7 @@
         <v>602</v>
       </c>
       <c r="C2" s="66">
-        <f t="shared" ref="C2" si="0">SUM(C4:C7)</f>
+        <f>SUM(C4:C7)</f>
         <v>1</v>
       </c>
       <c r="D2" s="66">
@@ -16534,143 +16517,143 @@
         <v>2</v>
       </c>
       <c r="E2" s="66">
-        <f t="shared" ref="E2:AM2" si="1">SUM(E3:E8)</f>
+        <f t="shared" ref="E2:AM2" si="0">SUM(E3:E8)</f>
         <v>2</v>
       </c>
       <c r="F2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
       <c r="G2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="M2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="N2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.75</v>
       </c>
       <c r="O2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="P2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="Q2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="S2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="T2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="U2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="V2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="W2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="X2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Y2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="Z2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AA2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AB2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AC2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="AD2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AE2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AF2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AG2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AH2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="AI2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="AJ2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="AK2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="AL2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="AM2" s="66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -16746,7 +16729,7 @@
       </c>
     </row>
     <row r="4" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="119" t="s">
         <v>605</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -16827,7 +16810,7 @@
       </c>
     </row>
     <row r="5" spans="1:39" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="118"/>
+      <c r="A5" s="120"/>
       <c r="B5" s="9" t="s">
         <v>909</v>
       </c>
@@ -16894,7 +16877,7 @@
       <c r="AM5" s="63"/>
     </row>
     <row r="6" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="118"/>
+      <c r="A6" s="120"/>
       <c r="B6" s="20" t="s">
         <v>910</v>
       </c>
@@ -16961,7 +16944,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="119"/>
+      <c r="A7" s="121"/>
       <c r="B7" s="9" t="s">
         <v>911</v>
       </c>
@@ -17096,11 +17079,6 @@
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -17643,19 +17621,19 @@
         <v>270</v>
       </c>
       <c r="D19" s="47" t="str">
-        <f t="shared" ref="D19" si="4">RIGHT(C19,5)</f>
+        <f>RIGHT(C19,5)</f>
         <v>04073</v>
       </c>
       <c r="E19" s="45">
-        <f t="shared" ref="E19" si="5">FIND(",",C19)+2</f>
+        <f>FIND(",",C19)+2</f>
         <v>10</v>
       </c>
       <c r="F19" s="45" t="str">
-        <f t="shared" ref="F19" si="6">MID(C19,E19,2)</f>
+        <f>MID(C19,E19,2)</f>
         <v>ME</v>
       </c>
       <c r="G19" s="45" t="str">
-        <f t="shared" ref="G19" si="7">MID(C19,1,E19-3)</f>
+        <f>MID(C19,1,E19-3)</f>
         <v>Sanford</v>
       </c>
       <c r="H19" s="59" t="s">
@@ -17723,26 +17701,26 @@
       </c>
     </row>
     <row r="22" spans="1:9" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="120" t="s">
+      <c r="A22" s="122" t="s">
         <v>953</v>
       </c>
-      <c r="B22" s="121"/>
-      <c r="C22" s="121"/>
-      <c r="D22" s="121"/>
-      <c r="E22" s="121"/>
-      <c r="F22" s="121"/>
-      <c r="G22" s="121"/>
-      <c r="H22" s="122"/>
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="123"/>
+      <c r="F22" s="123"/>
+      <c r="G22" s="123"/>
+      <c r="H22" s="124"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="123"/>
-      <c r="B23" s="124"/>
-      <c r="C23" s="124"/>
-      <c r="D23" s="124"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="124"/>
-      <c r="G23" s="124"/>
-      <c r="H23" s="125"/>
+      <c r="A23" s="125"/>
+      <c r="B23" s="126"/>
+      <c r="C23" s="126"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
+      <c r="F23" s="126"/>
+      <c r="G23" s="126"/>
+      <c r="H23" s="127"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="49" t="s">
@@ -17755,19 +17733,19 @@
         <v>262</v>
       </c>
       <c r="D24" s="86" t="str">
-        <f t="shared" ref="D24:D26" si="8">RIGHT(C24,5)</f>
+        <f>RIGHT(C24,5)</f>
         <v>12307</v>
       </c>
       <c r="E24" s="87">
-        <f t="shared" ref="E24:E26" si="9">FIND(",",C24)+2</f>
+        <f>FIND(",",C24)+2</f>
         <v>14</v>
       </c>
       <c r="F24" s="87" t="str">
-        <f t="shared" ref="F24:F26" si="10">MID(C24,E24,2)</f>
+        <f>MID(C24,E24,2)</f>
         <v>NY</v>
       </c>
       <c r="G24" s="87" t="str">
-        <f t="shared" ref="G24:G26" si="11">MID(C24,1,E24-3)</f>
+        <f>MID(C24,1,E24-3)</f>
         <v>Schenectady</v>
       </c>
       <c r="H24" s="58" t="s">
@@ -17785,19 +17763,19 @@
         <v>265</v>
       </c>
       <c r="D25" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f>RIGHT(C25,5)</f>
         <v>53081</v>
       </c>
       <c r="E25" s="87">
-        <f t="shared" si="9"/>
+        <f>FIND(",",C25)+2</f>
         <v>12</v>
       </c>
       <c r="F25" s="87" t="str">
-        <f t="shared" si="10"/>
+        <f>MID(C25,E25,2)</f>
         <v>WI</v>
       </c>
       <c r="G25" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f>MID(C25,1,E25-3)</f>
         <v>Sheboygan</v>
       </c>
       <c r="H25" s="58" t="s">
@@ -17815,19 +17793,19 @@
         <v>288</v>
       </c>
       <c r="D26" s="86" t="str">
-        <f t="shared" si="8"/>
+        <f>RIGHT(C26,5)</f>
         <v>49930</v>
       </c>
       <c r="E26" s="87">
-        <f t="shared" si="9"/>
+        <f>FIND(",",C26)+2</f>
         <v>10</v>
       </c>
       <c r="F26" s="87" t="str">
-        <f t="shared" si="10"/>
+        <f>MID(C26,E26,2)</f>
         <v>MI</v>
       </c>
       <c r="G26" s="87" t="str">
-        <f t="shared" si="11"/>
+        <f>MID(C26,1,E26-3)</f>
         <v>Hancock</v>
       </c>
       <c r="H26" s="57" t="s">
@@ -17901,11 +17879,6 @@
   <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -17914,7 +17887,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
@@ -18718,26 +18691,26 @@
       <c r="J27" s="96"/>
     </row>
     <row r="28" spans="1:10" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="120" t="s">
+      <c r="A28" s="122" t="s">
         <v>953</v>
       </c>
-      <c r="B28" s="121"/>
-      <c r="C28" s="121"/>
-      <c r="D28" s="121"/>
-      <c r="E28" s="121"/>
-      <c r="F28" s="121"/>
-      <c r="G28" s="121"/>
-      <c r="H28" s="122"/>
+      <c r="B28" s="123"/>
+      <c r="C28" s="123"/>
+      <c r="D28" s="123"/>
+      <c r="E28" s="123"/>
+      <c r="F28" s="123"/>
+      <c r="G28" s="123"/>
+      <c r="H28" s="124"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="123"/>
-      <c r="B29" s="124"/>
-      <c r="C29" s="124"/>
-      <c r="D29" s="124"/>
-      <c r="E29" s="124"/>
-      <c r="F29" s="124"/>
-      <c r="G29" s="124"/>
-      <c r="H29" s="125"/>
+      <c r="A29" s="125"/>
+      <c r="B29" s="126"/>
+      <c r="C29" s="126"/>
+      <c r="D29" s="126"/>
+      <c r="E29" s="126"/>
+      <c r="F29" s="126"/>
+      <c r="G29" s="126"/>
+      <c r="H29" s="127"/>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49" t="s">
@@ -18750,19 +18723,19 @@
         <v>265</v>
       </c>
       <c r="D31" s="86" t="str">
-        <f t="shared" ref="D31:D32" si="4">RIGHT(C31,5)</f>
+        <f>RIGHT(C31,5)</f>
         <v>53081</v>
       </c>
       <c r="E31" s="87">
-        <f t="shared" ref="E31:E32" si="5">FIND(",",C31)+2</f>
+        <f>FIND(",",C31)+2</f>
         <v>12</v>
       </c>
       <c r="F31" s="87" t="str">
-        <f t="shared" ref="F31:F32" si="6">MID(C31,E31,2)</f>
+        <f>MID(C31,E31,2)</f>
         <v>WI</v>
       </c>
       <c r="G31" s="87" t="str">
-        <f t="shared" ref="G31:G32" si="7">MID(C31,1,E31-3)</f>
+        <f>MID(C31,1,E31-3)</f>
         <v>Sheboygan</v>
       </c>
       <c r="H31" s="58" t="s">
@@ -18780,19 +18753,19 @@
         <v>288</v>
       </c>
       <c r="D32" s="86" t="str">
-        <f t="shared" si="4"/>
+        <f>RIGHT(C32,5)</f>
         <v>49930</v>
       </c>
       <c r="E32" s="87">
-        <f t="shared" si="5"/>
+        <f>FIND(",",C32)+2</f>
         <v>10</v>
       </c>
       <c r="F32" s="87" t="str">
-        <f t="shared" si="6"/>
+        <f>MID(C32,E32,2)</f>
         <v>MI</v>
       </c>
       <c r="G32" s="87" t="str">
-        <f t="shared" si="7"/>
+        <f>MID(C32,1,E32-3)</f>
         <v>Hancock</v>
       </c>
       <c r="H32" s="57" t="s">
@@ -18936,7 +18909,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18955,6 +18928,9 @@
       <c r="C1" s="53" t="s">
         <v>1006</v>
       </c>
+      <c r="D1" t="s">
+        <v>1011</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
@@ -18999,7 +18975,7 @@
       <c r="B4" s="109" t="s">
         <v>981</v>
       </c>
-      <c r="C4" s="126" t="s">
+      <c r="C4" s="116" t="s">
         <v>1008</v>
       </c>
       <c r="D4">
@@ -19024,7 +19000,7 @@
       <c r="E5" t="s">
         <v>612</v>
       </c>
-      <c r="F5" s="126" t="s">
+      <c r="F5" s="116" t="s">
         <v>1008</v>
       </c>
     </row>
@@ -19035,7 +19011,7 @@
       <c r="B6" s="109" t="s">
         <v>982</v>
       </c>
-      <c r="C6" s="126" t="s">
+      <c r="C6" s="116" t="s">
         <v>980</v>
       </c>
       <c r="D6">
@@ -19140,10 +19116,10 @@
       <c r="B12" s="109" t="s">
         <v>984</v>
       </c>
-      <c r="C12" s="126" t="s">
+      <c r="C12" s="116" t="s">
         <v>1005</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="117">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -19191,7 +19167,7 @@
       <c r="B15" s="109" t="s">
         <v>985</v>
       </c>
-      <c r="C15" s="126" t="s">
+      <c r="C15" s="116" t="s">
         <v>1010</v>
       </c>
       <c r="D15">
@@ -19242,7 +19218,7 @@
       <c r="B18" s="48" t="s">
         <v>878</v>
       </c>
-      <c r="C18" s="126" t="s">
+      <c r="C18" s="116" t="s">
         <v>26</v>
       </c>
       <c r="D18">
@@ -19311,7 +19287,7 @@
       <c r="B22" s="48" t="s">
         <v>988</v>
       </c>
-      <c r="C22" s="126" t="s">
+      <c r="C22" s="116" t="s">
         <v>987</v>
       </c>
       <c r="D22">
@@ -19326,7 +19302,7 @@
       <c r="B23" s="109" t="s">
         <v>986</v>
       </c>
-      <c r="C23" s="126" t="s">
+      <c r="C23" s="116" t="s">
         <v>990</v>
       </c>
       <c r="D23">

</xml_diff>